<commit_message>
set property's private value as true
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Struct/IObject.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Struct/IObject.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvsheng.huang\Desktop\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Excel_Struct\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView windowWidth="19560" windowHeight="8460"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="8460"/>
   </bookViews>
   <sheets>
     <sheet name="Property" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <extLst/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>Id</t>
   </si>
@@ -77,17 +81,17 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="宋体"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <name val="宋体"/>
       <family val="2"/>
       <charset val="134"/>
@@ -110,23 +114,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -138,14 +127,19 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
-    <cellStyle name="货币" xfId="2" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="3" builtinId="6"/>
-    <cellStyle name="百分比" xfId="4" builtinId="5"/>
-    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -444,6 +438,7 @@
           </a:gdLst>
           <a:ahLst/>
           <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
           <a:pathLst>
             <a:path w="21600" h="21600"/>
           </a:pathLst>
@@ -476,15 +471,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F6"/>
+      <selection activeCell="D2" sqref="D2:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10.5" customWidth="1"/>
     <col min="2" max="2" width="8.25" customWidth="1"/>
@@ -497,7 +491,7 @@
     <col min="10" max="10" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -529,7 +523,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -540,7 +534,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
@@ -559,7 +553,7 @@
       </c>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -570,7 +564,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" t="b">
         <v>0</v>
@@ -589,7 +583,7 @@
       </c>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -600,7 +594,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
@@ -619,7 +613,7 @@
       </c>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>16</v>
       </c>
@@ -630,7 +624,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" t="b">
         <v>0</v>
@@ -651,7 +645,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -662,7 +656,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="b">
         <v>0</v>
@@ -682,14 +676,15 @@
       <c r="J6" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F6 F7:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576 D2:D6">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>